<commit_message>
fix : latest sum
</commit_message>
<xml_diff>
--- a/For Bank (August).xlsx
+++ b/For Bank (August).xlsx
@@ -1783,7 +1783,7 @@
   </sheetPr>
   <dimension ref="A1:K213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>45496</v>
+        <v>45130</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>

</xml_diff>